<commit_message>
Update data from Streamlit app
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,20 +556,20 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
+        <v>45504</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>45869</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>46234</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>250000000</v>
+        <v>235000000</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>235000000</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -586,20 +586,20 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
+        <v>45152</v>
+      </c>
+      <c r="C5" s="2" t="n">
         <v>45883</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>46248</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>215000000</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>215000000</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -616,10 +616,10 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
+        <v>45528</v>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>45893</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>46258</v>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
@@ -629,7 +629,7 @@
         <v>250000000</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>250000000</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -646,20 +646,20 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
+        <v>45572</v>
+      </c>
+      <c r="C7" s="2" t="n">
         <v>45937</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>46667</v>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>375000000</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>375000000</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -676,24 +676,24 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
+        <v>44843</v>
+      </c>
+      <c r="C8" s="2" t="n">
         <v>45939</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>46669</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
-        <v>140000000</v>
+        <v>160000000</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>160000000</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Full Lease Upfront</t>
+          <t>Split Per Year</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
@@ -736,20 +736,24 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
+        <v>44726</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>45822</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>46918</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Reminder: Lease Ending Soon</t>
+        </is>
+      </c>
       <c r="E10" t="n">
         <v>3</v>
       </c>
       <c r="F10" t="n">
-        <v>70000000</v>
+        <v>75000000</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>75000000</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -766,20 +770,20 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
+        <v>45260</v>
+      </c>
+      <c r="C11" s="2" t="n">
         <v>45991</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>47087</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>75000000</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>75000000</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -796,10 +800,10 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
+        <v>45291</v>
+      </c>
+      <c r="C12" s="2" t="n">
         <v>46022</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>46752</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
@@ -809,7 +813,7 @@
         <v>525000000</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>525000000</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -826,28 +830,156 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
+        <v>45657</v>
+      </c>
+      <c r="C13" s="2" t="n">
         <v>46022</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>46752</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>180000000</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>180000000</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Split Per Year</t>
+          <t>Full Lease Upfront</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>PT Mandiri Akur Pratama (Jogja)</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>45339</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>46070</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="n">
+        <v>190000000</v>
+      </c>
+      <c r="G14" t="n">
+        <v>190000000</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Full Lease Upfront</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PT Tiki JNE </t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>45108</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>46569</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+      <c r="F15" t="n">
+        <v>195000000</v>
+      </c>
+      <c r="G15" t="n">
+        <v>195000000</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Full Lease Upfront</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>PT Mandiri Utama Finance</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>44166</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>5</v>
+      </c>
+      <c r="F16" t="n">
+        <v>235000000</v>
+      </c>
+      <c r="G16" t="n">
+        <v>235000000</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Custom Split</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>50/50/0/0/0</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PT Kawan Lama Solusi (Krisbow)</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>45624</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>47450</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F17" t="n">
+        <v>213750000</v>
+      </c>
+      <c r="G17" t="n">
+        <v>213750000</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Custom Split</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>60/0/40/0/0</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>